<commit_message>
_ modifs code industrie pour débugage
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/parameters.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Industry_model/Input/Steel/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1B879D-21DC-F94E-9919-3B6ED2B7A6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5295C45C-994C-4C20-B7B0-289AA312285B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="1900" windowWidth="20340" windowHeight="12180" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
+    <workbookView xWindow="2295" yWindow="1905" windowWidth="20340" windowHeight="12180" activeTab="1" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
   </bookViews>
   <sheets>
     <sheet name="TECHNOLOGIES" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Scrap</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>forced_resource</t>
-  </si>
-  <si>
-    <t>rajouté</t>
   </si>
   <si>
     <t>RESOURCES</t>
@@ -665,18 +662,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEC0513-801E-2542-89D6-117D6191FB3E}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -708,7 +705,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +716,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -733,7 +730,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -763,7 +760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -787,7 +784,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -810,7 +807,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -836,7 +833,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -856,7 +853,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -879,7 +876,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -902,7 +899,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -925,7 +922,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -936,12 +933,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -949,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -972,7 +969,7 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -989,7 +986,7 @@
         <v>0.16274539488251155</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>35</v>
       </c>
@@ -1020,13 +1017,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7586E3A9-C0EE-6F42-8EFF-5D7691C2A1FF}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>39</v>
@@ -1044,7 +1043,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1116,11 +1115,8 @@
       <c r="C6" s="4">
         <v>291.66900000000004</v>
       </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>30</v>
       </c>
@@ -1148,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1162,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1176,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
@@ -1190,7 +1186,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
@@ -1204,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>29</v>
       </c>
@@ -1231,12 +1227,12 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1273,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
@@ -1296,7 +1292,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
@@ -1307,7 +1303,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>24</v>
       </c>
@@ -1318,7 +1314,7 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
@@ -1327,7 +1323,7 @@
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>35</v>
       </c>
@@ -1335,7 +1331,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1346,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1364,7 +1360,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1384,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1407,7 +1403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1430,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1448,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1468,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1485,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1505,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
_ modifs code industrie + paramètres d'entrée
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/parameters.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Industry_model/Input/Steel/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2AD0E3-3502-A44A-9C3D-476B4FE75E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2523425-693F-4A1A-927C-B422826AD52E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="500" windowWidth="23740" windowHeight="11760" activeTab="1" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
+    <workbookView xWindow="5052" yWindow="492" windowWidth="23748" windowHeight="11760" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
   </bookViews>
   <sheets>
     <sheet name="TECHNOLOGIES" sheetId="1" r:id="rId1"/>
@@ -22,20 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Scrap</t>
   </si>
@@ -167,6 +159,9 @@
   </si>
   <si>
     <t>RESOURCES</t>
+  </si>
+  <si>
+    <t>is_product</t>
   </si>
 </sst>
 </file>
@@ -316,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -340,6 +335,8 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,18 +653,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEC0513-801E-2542-89D6-117D6191FB3E}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.09765625" customWidth="1"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -699,7 +696,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,7 +707,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -724,7 +721,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -746,15 +743,8 @@
       <c r="G4">
         <v>53.2</v>
       </c>
-      <c r="H4" s="7">
-        <v>0.66</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -776,9 +766,15 @@
       <c r="G5">
         <v>53.2</v>
       </c>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -801,7 +797,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -827,7 +823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -847,7 +843,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -870,7 +866,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -893,7 +889,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -916,7 +912,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -924,23 +920,29 @@
         <v>-1</v>
       </c>
       <c r="G12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -948,7 +950,7 @@
         <v>12.13</v>
       </c>
       <c r="C15">
-        <v>3448.3536819299948</v>
+        <v>1800</v>
       </c>
       <c r="D15">
         <v>25</v>
@@ -963,12 +965,12 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -980,7 +982,7 @@
         <v>0.16274539488251155</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>33</v>
       </c>
@@ -1009,15 +1011,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7586E3A9-C0EE-6F42-8EFF-5D7691C2A1FF}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
@@ -1027,17 +1029,20 @@
       <c r="C1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1049,11 +1054,14 @@
         <f>250*0.95</f>
         <v>237.5</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="24">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -1064,11 +1072,14 @@
       <c r="C3" s="8">
         <v>400</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1080,11 +1091,14 @@
         <f>60*17.8</f>
         <v>1068</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1094,11 +1108,14 @@
       <c r="C5" s="4">
         <v>60</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="24">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1109,8 +1126,11 @@
       <c r="C6" s="4">
         <v>291.66900000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1118,13 +1138,16 @@
         <v>-1</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>30</v>
       </c>
@@ -1132,13 +1155,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="15">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10000</v>
+      </c>
+      <c r="D8" s="24">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1146,13 +1172,16 @@
         <v>0</v>
       </c>
       <c r="C9" s="15">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="24">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1162,11 +1191,14 @@
       <c r="C10" s="13">
         <v>1.5</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="24">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
@@ -1174,16 +1206,16 @@
         <v>0</v>
       </c>
       <c r="C11" s="15">
-        <v>0</v>
-      </c>
-      <c r="D11">
+        <v>10000</v>
+      </c>
+      <c r="D11" s="24">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>15000000</v>
       </c>
-      <c r="F11">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
@@ -1191,13 +1223,16 @@
         <v>0</v>
       </c>
       <c r="C12" s="5">
-        <v>10000000</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10000</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>29</v>
       </c>
@@ -1205,9 +1240,12 @@
         <v>0</v>
       </c>
       <c r="C13" s="6">
-        <v>10000000</v>
-      </c>
-      <c r="D13">
+        <v>10000</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>0</v>
       </c>
     </row>
@@ -1221,15 +1259,15 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:K17"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1270,7 +1308,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -1278,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
@@ -1288,8 +1326,11 @@
       <c r="I3">
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
@@ -1299,28 +1340,37 @@
       <c r="I4">
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="4">
         <v>3.04</v>
       </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
       <c r="I5" s="4">
         <v>4.45</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
+      <c r="E6">
+        <v>55</v>
+      </c>
       <c r="H6" s="4">
-        <v>55</v>
+        <v>-1</v>
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>33</v>
       </c>
@@ -1328,7 +1378,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1343,7 +1393,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1357,7 +1407,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1377,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1400,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1423,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1441,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1461,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1478,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1498,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
_ Mise à jour modèle sans planification   * Modification des contraintes associées au paramètre P_forced_prod_ratio par la transformation de celui-ci en une valeur min et max   * La production pour la technologie associée est donc contenue entre ces deux valeurs
_ Mise à jour en conséquence du fichier Excel d'entrée
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/parameters.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2523425-693F-4A1A-927C-B422826AD52E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D44D933-E557-4A6D-9938-4E633D3E8360}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5052" yWindow="492" windowWidth="23748" windowHeight="11760" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>Scrap</t>
   </si>
@@ -143,9 +143,6 @@
     <t>emissions_r</t>
   </si>
   <si>
-    <t>forced_prod_ratio</t>
-  </si>
-  <si>
     <t>max_capacity_t</t>
   </si>
   <si>
@@ -162,6 +159,12 @@
   </si>
   <si>
     <t>is_product</t>
+  </si>
+  <si>
+    <t>forced_prod_ratio_min</t>
+  </si>
+  <si>
+    <t>forced_prod_ratio_max</t>
   </si>
 </sst>
 </file>
@@ -651,20 +654,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEC0513-801E-2542-89D6-117D6191FB3E}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.09765625" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
-    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="8" max="9" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -687,16 +690,19 @@
         <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,9 +711,10 @@
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2" s="7"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -719,9 +726,10 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3" s="7"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -743,8 +751,18 @@
       <c r="G4">
         <v>53.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -766,15 +784,8 @@
       <c r="G5">
         <v>53.2</v>
       </c>
-      <c r="H5" s="7">
-        <v>0.66</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -797,7 +808,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -817,13 +828,16 @@
         <v>53.2</v>
       </c>
       <c r="H7" s="16">
-        <v>0.34</v>
-      </c>
-      <c r="J7" s="17" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -843,7 +857,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -866,7 +880,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -889,7 +903,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -912,7 +926,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -923,7 +937,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -931,7 +945,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -942,7 +956,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -965,7 +979,7 @@
         <v>324.97573965832413</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -982,7 +996,7 @@
         <v>0.16274539488251155</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>33</v>
       </c>
@@ -997,10 +1011,10 @@
         <f>49.2578*13</f>
         <v>640.35140000000001</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>860000</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1021,7 +1035,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>37</v>
@@ -1030,16 +1044,16 @@
         <v>34</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>